<commit_message>
forgot to commit for a long time
</commit_message>
<xml_diff>
--- a/plate_info/SummaryAnalizedPlates.xlsx
+++ b/plate_info/SummaryAnalizedPlates.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\coren\Documents\WUR\MsC Thesis\code\plate_info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9F4167-2755-46F8-B0A2-FE708A50B43C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C7131A-D4D0-4B91-9805-5235DFF878A8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82D79ED9-50EF-C049-AB06-E57D2479A472}"/>
   </bookViews>
@@ -623,7 +623,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -877,6 +877,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -972,8 +973,8 @@
       <sheetName val="qPCR 1P 100N"/>
       <sheetName val="qPCR 100P 100N"/>
       <sheetName val="CrossingStats"/>
+      <sheetName val="DoNotChange"/>
       <sheetName val="18.09.19 Plate pictures"/>
-      <sheetName val="DoNotChange"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
@@ -7041,7 +7042,7 @@
         </row>
       </sheetData>
       <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
+      <sheetData sheetId="6" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -7344,10 +7345,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A272A16E-E3F9-384D-9E29-D88BCF4CFB49}">
-  <dimension ref="B1:AK77"/>
+  <dimension ref="B1:AK78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -7363,136 +7364,136 @@
   <sheetData>
     <row r="1" spans="2:37" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:37" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G2" s="110" t="s">
+      <c r="G2" s="111" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="111"/>
-      <c r="I2" s="111"/>
-      <c r="J2" s="111"/>
-      <c r="K2" s="111"/>
-      <c r="L2" s="111"/>
-      <c r="M2" s="111"/>
-      <c r="N2" s="111"/>
-      <c r="O2" s="111"/>
-      <c r="P2" s="111"/>
-      <c r="Q2" s="111"/>
-      <c r="R2" s="111"/>
-      <c r="S2" s="111"/>
-      <c r="T2" s="111"/>
-      <c r="U2" s="111"/>
-      <c r="V2" s="111"/>
-      <c r="W2" s="111"/>
-      <c r="X2" s="111"/>
-      <c r="Y2" s="111"/>
-      <c r="Z2" s="111"/>
-      <c r="AA2" s="111"/>
-      <c r="AB2" s="111"/>
-      <c r="AC2" s="111"/>
-      <c r="AD2" s="112"/>
+      <c r="H2" s="112"/>
+      <c r="I2" s="112"/>
+      <c r="J2" s="112"/>
+      <c r="K2" s="112"/>
+      <c r="L2" s="112"/>
+      <c r="M2" s="112"/>
+      <c r="N2" s="112"/>
+      <c r="O2" s="112"/>
+      <c r="P2" s="112"/>
+      <c r="Q2" s="112"/>
+      <c r="R2" s="112"/>
+      <c r="S2" s="112"/>
+      <c r="T2" s="112"/>
+      <c r="U2" s="112"/>
+      <c r="V2" s="112"/>
+      <c r="W2" s="112"/>
+      <c r="X2" s="112"/>
+      <c r="Y2" s="112"/>
+      <c r="Z2" s="112"/>
+      <c r="AA2" s="112"/>
+      <c r="AB2" s="112"/>
+      <c r="AC2" s="112"/>
+      <c r="AD2" s="113"/>
     </row>
     <row r="3" spans="2:37" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G3" s="113" t="s">
+      <c r="G3" s="114" t="s">
         <v>36</v>
       </c>
-      <c r="H3" s="114"/>
-      <c r="I3" s="114"/>
-      <c r="J3" s="114"/>
-      <c r="K3" s="114"/>
-      <c r="L3" s="114"/>
-      <c r="M3" s="114"/>
-      <c r="N3" s="114"/>
-      <c r="O3" s="113" t="s">
+      <c r="H3" s="115"/>
+      <c r="I3" s="115"/>
+      <c r="J3" s="115"/>
+      <c r="K3" s="115"/>
+      <c r="L3" s="115"/>
+      <c r="M3" s="115"/>
+      <c r="N3" s="115"/>
+      <c r="O3" s="114" t="s">
         <v>3</v>
       </c>
-      <c r="P3" s="114"/>
-      <c r="Q3" s="114"/>
-      <c r="R3" s="114"/>
-      <c r="S3" s="114"/>
-      <c r="T3" s="114"/>
-      <c r="U3" s="114"/>
-      <c r="V3" s="114"/>
-      <c r="W3" s="107" t="s">
+      <c r="P3" s="115"/>
+      <c r="Q3" s="115"/>
+      <c r="R3" s="115"/>
+      <c r="S3" s="115"/>
+      <c r="T3" s="115"/>
+      <c r="U3" s="115"/>
+      <c r="V3" s="115"/>
+      <c r="W3" s="108" t="s">
         <v>30</v>
       </c>
-      <c r="X3" s="108"/>
-      <c r="Y3" s="108"/>
-      <c r="Z3" s="108"/>
-      <c r="AA3" s="108"/>
-      <c r="AB3" s="108"/>
-      <c r="AC3" s="108"/>
-      <c r="AD3" s="109"/>
+      <c r="X3" s="109"/>
+      <c r="Y3" s="109"/>
+      <c r="Z3" s="109"/>
+      <c r="AA3" s="109"/>
+      <c r="AB3" s="109"/>
+      <c r="AC3" s="109"/>
+      <c r="AD3" s="110"/>
     </row>
     <row r="4" spans="2:37" ht="34.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="101" t="s">
+      <c r="B4" s="102" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="103" t="s">
+      <c r="C4" s="104" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="103" t="s">
+      <c r="D4" s="104" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="103" t="s">
+      <c r="E4" s="104" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="105" t="s">
+      <c r="F4" s="106" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="100" t="s">
+      <c r="G4" s="101" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="98"/>
-      <c r="I4" s="97" t="s">
+      <c r="H4" s="99"/>
+      <c r="I4" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="98"/>
-      <c r="K4" s="97" t="s">
+      <c r="J4" s="99"/>
+      <c r="K4" s="98" t="s">
         <v>26</v>
       </c>
-      <c r="L4" s="98"/>
-      <c r="M4" s="97" t="s">
+      <c r="L4" s="99"/>
+      <c r="M4" s="98" t="s">
         <v>27</v>
       </c>
-      <c r="N4" s="115"/>
-      <c r="O4" s="100" t="s">
+      <c r="N4" s="116"/>
+      <c r="O4" s="101" t="s">
         <v>4</v>
       </c>
-      <c r="P4" s="98"/>
-      <c r="Q4" s="97" t="s">
+      <c r="P4" s="99"/>
+      <c r="Q4" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="R4" s="98"/>
-      <c r="S4" s="97" t="s">
+      <c r="R4" s="99"/>
+      <c r="S4" s="98" t="s">
         <v>26</v>
       </c>
-      <c r="T4" s="98"/>
-      <c r="U4" s="97" t="s">
+      <c r="T4" s="99"/>
+      <c r="U4" s="98" t="s">
         <v>27</v>
       </c>
-      <c r="V4" s="99"/>
-      <c r="W4" s="115" t="s">
+      <c r="V4" s="100"/>
+      <c r="W4" s="116" t="s">
         <v>4</v>
       </c>
-      <c r="X4" s="98"/>
-      <c r="Y4" s="97" t="s">
+      <c r="X4" s="99"/>
+      <c r="Y4" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="Z4" s="98"/>
-      <c r="AA4" s="97" t="s">
+      <c r="Z4" s="99"/>
+      <c r="AA4" s="98" t="s">
         <v>26</v>
       </c>
-      <c r="AB4" s="98"/>
-      <c r="AC4" s="97" t="s">
+      <c r="AB4" s="99"/>
+      <c r="AC4" s="98" t="s">
         <v>27</v>
       </c>
-      <c r="AD4" s="99"/>
+      <c r="AD4" s="100"/>
     </row>
     <row r="5" spans="2:37" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="102"/>
-      <c r="C5" s="104"/>
-      <c r="D5" s="104"/>
-      <c r="E5" s="104"/>
-      <c r="F5" s="106"/>
+      <c r="B5" s="103"/>
+      <c r="C5" s="105"/>
+      <c r="D5" s="105"/>
+      <c r="E5" s="105"/>
+      <c r="F5" s="107"/>
       <c r="G5" s="14" t="s">
         <v>24</v>
       </c>
@@ -7697,16 +7698,16 @@
       <c r="AB7" s="34"/>
       <c r="AC7" s="10"/>
       <c r="AD7" s="20"/>
-      <c r="AF7" s="117" t="s">
+      <c r="AF7" s="118" t="s">
         <v>12</v>
       </c>
-      <c r="AG7" s="116" t="s">
+      <c r="AG7" s="117" t="s">
         <v>11</v>
       </c>
-      <c r="AH7" s="116"/>
-      <c r="AI7" s="116"/>
-      <c r="AJ7" s="116"/>
-      <c r="AK7" s="116"/>
+      <c r="AH7" s="117"/>
+      <c r="AI7" s="117"/>
+      <c r="AJ7" s="117"/>
+      <c r="AK7" s="117"/>
     </row>
     <row r="8" spans="2:37" x14ac:dyDescent="0.3">
       <c r="B8" s="36">
@@ -7774,14 +7775,14 @@
       <c r="AB8" s="34"/>
       <c r="AC8" s="10"/>
       <c r="AD8" s="20"/>
-      <c r="AF8" s="117"/>
-      <c r="AG8" s="116" t="s">
+      <c r="AF8" s="118"/>
+      <c r="AG8" s="117" t="s">
         <v>13</v>
       </c>
-      <c r="AH8" s="116"/>
-      <c r="AI8" s="116"/>
-      <c r="AJ8" s="116"/>
-      <c r="AK8" s="116"/>
+      <c r="AH8" s="117"/>
+      <c r="AI8" s="117"/>
+      <c r="AJ8" s="117"/>
+      <c r="AK8" s="117"/>
     </row>
     <row r="9" spans="2:37" x14ac:dyDescent="0.3">
       <c r="B9" s="36">
@@ -7845,14 +7846,14 @@
       <c r="AB9" s="34"/>
       <c r="AC9" s="10"/>
       <c r="AD9" s="20"/>
-      <c r="AF9" s="117"/>
-      <c r="AG9" s="116" t="s">
+      <c r="AF9" s="118"/>
+      <c r="AG9" s="117" t="s">
         <v>14</v>
       </c>
-      <c r="AH9" s="116"/>
-      <c r="AI9" s="116"/>
-      <c r="AJ9" s="116"/>
-      <c r="AK9" s="116"/>
+      <c r="AH9" s="117"/>
+      <c r="AI9" s="117"/>
+      <c r="AJ9" s="117"/>
+      <c r="AK9" s="117"/>
     </row>
     <row r="10" spans="2:37" x14ac:dyDescent="0.3">
       <c r="B10" s="36">
@@ -9930,24 +9931,24 @@
       <c r="AD50" s="10"/>
     </row>
     <row r="51" spans="2:35" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G51" s="110" t="s">
+      <c r="G51" s="111" t="s">
         <v>29</v>
       </c>
-      <c r="H51" s="111"/>
-      <c r="I51" s="111"/>
-      <c r="J51" s="111"/>
-      <c r="K51" s="111"/>
-      <c r="L51" s="111"/>
-      <c r="M51" s="111"/>
-      <c r="N51" s="111"/>
-      <c r="O51" s="111"/>
-      <c r="P51" s="111"/>
-      <c r="Q51" s="111"/>
-      <c r="R51" s="111"/>
-      <c r="S51" s="111"/>
-      <c r="T51" s="111"/>
-      <c r="U51" s="111"/>
-      <c r="V51" s="112"/>
+      <c r="H51" s="112"/>
+      <c r="I51" s="112"/>
+      <c r="J51" s="112"/>
+      <c r="K51" s="112"/>
+      <c r="L51" s="112"/>
+      <c r="M51" s="112"/>
+      <c r="N51" s="112"/>
+      <c r="O51" s="112"/>
+      <c r="P51" s="112"/>
+      <c r="Q51" s="112"/>
+      <c r="R51" s="112"/>
+      <c r="S51" s="112"/>
+      <c r="T51" s="112"/>
+      <c r="U51" s="112"/>
+      <c r="V51" s="113"/>
       <c r="W51" s="44"/>
       <c r="X51" s="44"/>
       <c r="Y51" s="44"/>
@@ -9963,26 +9964,26 @@
       <c r="AI51" s="10"/>
     </row>
     <row r="52" spans="2:35" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G52" s="107" t="s">
+      <c r="G52" s="108" t="s">
         <v>2</v>
       </c>
-      <c r="H52" s="108"/>
-      <c r="I52" s="108"/>
-      <c r="J52" s="108"/>
-      <c r="K52" s="108"/>
-      <c r="L52" s="108"/>
-      <c r="M52" s="108"/>
-      <c r="N52" s="109"/>
-      <c r="O52" s="108" t="s">
+      <c r="H52" s="109"/>
+      <c r="I52" s="109"/>
+      <c r="J52" s="109"/>
+      <c r="K52" s="109"/>
+      <c r="L52" s="109"/>
+      <c r="M52" s="109"/>
+      <c r="N52" s="110"/>
+      <c r="O52" s="109" t="s">
         <v>31</v>
       </c>
-      <c r="P52" s="108"/>
-      <c r="Q52" s="108"/>
-      <c r="R52" s="108"/>
-      <c r="S52" s="108"/>
-      <c r="T52" s="108"/>
-      <c r="U52" s="108"/>
-      <c r="V52" s="109"/>
+      <c r="P52" s="109"/>
+      <c r="Q52" s="109"/>
+      <c r="R52" s="109"/>
+      <c r="S52" s="109"/>
+      <c r="T52" s="109"/>
+      <c r="U52" s="109"/>
+      <c r="V52" s="110"/>
       <c r="W52" s="5"/>
       <c r="X52" s="5"/>
       <c r="Y52" s="5"/>
@@ -9998,60 +9999,60 @@
       <c r="AI52" s="10"/>
     </row>
     <row r="53" spans="2:35" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B53" s="101" t="s">
+      <c r="B53" s="102" t="s">
         <v>6</v>
       </c>
-      <c r="C53" s="103" t="s">
+      <c r="C53" s="104" t="s">
         <v>7</v>
       </c>
-      <c r="D53" s="103" t="s">
+      <c r="D53" s="104" t="s">
         <v>35</v>
       </c>
-      <c r="E53" s="103" t="s">
+      <c r="E53" s="104" t="s">
         <v>1</v>
       </c>
-      <c r="F53" s="105" t="s">
+      <c r="F53" s="106" t="s">
         <v>8</v>
       </c>
-      <c r="G53" s="100" t="s">
+      <c r="G53" s="101" t="s">
         <v>4</v>
       </c>
-      <c r="H53" s="98"/>
-      <c r="I53" s="97" t="s">
+      <c r="H53" s="99"/>
+      <c r="I53" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="J53" s="98"/>
-      <c r="K53" s="97" t="s">
+      <c r="J53" s="99"/>
+      <c r="K53" s="98" t="s">
         <v>26</v>
       </c>
-      <c r="L53" s="98"/>
-      <c r="M53" s="97" t="s">
+      <c r="L53" s="99"/>
+      <c r="M53" s="98" t="s">
         <v>27</v>
       </c>
-      <c r="N53" s="99"/>
-      <c r="O53" s="100" t="s">
+      <c r="N53" s="100"/>
+      <c r="O53" s="101" t="s">
         <v>4</v>
       </c>
-      <c r="P53" s="98"/>
-      <c r="Q53" s="97" t="s">
+      <c r="P53" s="99"/>
+      <c r="Q53" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="R53" s="98"/>
-      <c r="S53" s="97" t="s">
+      <c r="R53" s="99"/>
+      <c r="S53" s="98" t="s">
         <v>26</v>
       </c>
-      <c r="T53" s="98"/>
-      <c r="U53" s="97" t="s">
+      <c r="T53" s="99"/>
+      <c r="U53" s="98" t="s">
         <v>27</v>
       </c>
-      <c r="V53" s="99"/>
+      <c r="V53" s="100"/>
     </row>
     <row r="54" spans="2:35" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B54" s="102"/>
-      <c r="C54" s="104"/>
-      <c r="D54" s="104"/>
-      <c r="E54" s="104"/>
-      <c r="F54" s="106"/>
+      <c r="B54" s="103"/>
+      <c r="C54" s="105"/>
+      <c r="D54" s="105"/>
+      <c r="E54" s="105"/>
+      <c r="F54" s="107"/>
       <c r="G54" s="16" t="s">
         <v>24</v>
       </c>
@@ -10201,40 +10202,32 @@
     </row>
     <row r="57" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B57" s="36">
-        <v>102</v>
+        <v>59</v>
       </c>
       <c r="C57" s="8">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D57" s="39">
         <v>25</v>
       </c>
-      <c r="E57" s="49">
-        <v>44191</v>
+      <c r="E57" s="97">
+        <v>44161</v>
       </c>
       <c r="F57" s="57">
-        <v>44178</v>
-      </c>
-      <c r="G57" s="61" t="s">
-        <v>9</v>
-      </c>
-      <c r="H57" s="7" t="s">
-        <v>9</v>
-      </c>
+        <v>44183</v>
+      </c>
+      <c r="G57" s="61"/>
+      <c r="H57" s="7"/>
       <c r="I57" s="25"/>
       <c r="J57" s="29"/>
       <c r="K57" s="8"/>
       <c r="L57" s="30"/>
       <c r="M57" s="8"/>
       <c r="N57" s="9"/>
-      <c r="O57" s="60" t="s">
-        <v>9</v>
-      </c>
-      <c r="P57" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q57" s="26"/>
-      <c r="R57" s="30"/>
+      <c r="O57" s="73"/>
+      <c r="P57" s="29"/>
+      <c r="Q57" s="25"/>
+      <c r="R57" s="29"/>
       <c r="S57" s="8"/>
       <c r="T57" s="34"/>
       <c r="U57" s="10"/>
@@ -10242,19 +10235,19 @@
     </row>
     <row r="58" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B58" s="36">
-        <v>38</v>
+        <v>102</v>
       </c>
       <c r="C58" s="8">
-        <v>29</v>
-      </c>
-      <c r="D58" s="39" t="s">
-        <v>34</v>
+        <v>40</v>
+      </c>
+      <c r="D58" s="39">
+        <v>25</v>
       </c>
       <c r="E58" s="49">
-        <v>44167</v>
+        <v>44191</v>
       </c>
       <c r="F58" s="57">
-        <v>44187</v>
+        <v>44209</v>
       </c>
       <c r="G58" s="61" t="s">
         <v>9</v>
@@ -10274,7 +10267,7 @@
       <c r="P58" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="Q58" s="8"/>
+      <c r="Q58" s="26"/>
       <c r="R58" s="30"/>
       <c r="S58" s="8"/>
       <c r="T58" s="34"/>
@@ -10283,10 +10276,10 @@
     </row>
     <row r="59" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B59" s="36">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="C59" s="8">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D59" s="39" t="s">
         <v>34</v>
@@ -10324,19 +10317,19 @@
     </row>
     <row r="60" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B60" s="36">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="C60" s="8">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D60" s="39" t="s">
         <v>34</v>
       </c>
       <c r="E60" s="49">
-        <v>44169</v>
+        <v>44167</v>
       </c>
       <c r="F60" s="57">
-        <v>44189</v>
+        <v>44187</v>
       </c>
       <c r="G60" s="61" t="s">
         <v>9</v>
@@ -10344,12 +10337,8 @@
       <c r="H60" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="I60" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="J60" s="29" t="s">
-        <v>9</v>
-      </c>
+      <c r="I60" s="25"/>
+      <c r="J60" s="29"/>
       <c r="K60" s="8"/>
       <c r="L60" s="30"/>
       <c r="M60" s="8"/>
@@ -10360,12 +10349,8 @@
       <c r="P60" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="Q60" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="R60" s="29" t="s">
-        <v>9</v>
-      </c>
+      <c r="Q60" s="8"/>
+      <c r="R60" s="30"/>
       <c r="S60" s="8"/>
       <c r="T60" s="34"/>
       <c r="U60" s="10"/>
@@ -10373,10 +10358,10 @@
     </row>
     <row r="61" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B61" s="36">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="C61" s="8">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D61" s="39" t="s">
         <v>34</v>
@@ -10422,19 +10407,19 @@
     </row>
     <row r="62" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B62" s="36">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="C62" s="8">
-        <v>22</v>
-      </c>
-      <c r="D62" s="39">
-        <v>30</v>
-      </c>
-      <c r="E62" s="70">
-        <v>44172</v>
-      </c>
-      <c r="F62" s="71">
-        <v>44192</v>
+        <v>24</v>
+      </c>
+      <c r="D62" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="E62" s="49">
+        <v>44169</v>
+      </c>
+      <c r="F62" s="57">
+        <v>44189</v>
       </c>
       <c r="G62" s="61" t="s">
         <v>9</v>
@@ -10471,19 +10456,19 @@
     </row>
     <row r="63" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B63" s="36">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="C63" s="8">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="D63" s="39">
-        <v>35</v>
-      </c>
-      <c r="E63" s="49">
-        <v>44179</v>
-      </c>
-      <c r="F63" s="57">
-        <v>44200</v>
+        <v>30</v>
+      </c>
+      <c r="E63" s="70">
+        <v>44172</v>
+      </c>
+      <c r="F63" s="71">
+        <v>44192</v>
       </c>
       <c r="G63" s="61" t="s">
         <v>9</v>
@@ -10491,8 +10476,12 @@
       <c r="H63" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="I63" s="25"/>
-      <c r="J63" s="29"/>
+      <c r="I63" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="J63" s="29" t="s">
+        <v>9</v>
+      </c>
       <c r="K63" s="8"/>
       <c r="L63" s="30"/>
       <c r="M63" s="8"/>
@@ -10503,8 +10492,12 @@
       <c r="P63" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="Q63" s="8"/>
-      <c r="R63" s="30"/>
+      <c r="Q63" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="R63" s="29" t="s">
+        <v>9</v>
+      </c>
       <c r="S63" s="8"/>
       <c r="T63" s="34"/>
       <c r="U63" s="10"/>
@@ -10512,10 +10505,10 @@
     </row>
     <row r="64" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B64" s="36">
-        <v>126</v>
+        <v>66</v>
       </c>
       <c r="C64" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D64" s="39">
         <v>35</v>
@@ -10552,14 +10545,14 @@
       <c r="V64" s="20"/>
     </row>
     <row r="65" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B65" s="75">
-        <v>13</v>
+      <c r="B65" s="36">
+        <v>126</v>
       </c>
       <c r="C65" s="8">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D65" s="39">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="E65" s="49">
         <v>44179</v>
@@ -10567,16 +10560,24 @@
       <c r="F65" s="57">
         <v>44200</v>
       </c>
-      <c r="G65" s="6"/>
-      <c r="H65" s="7"/>
+      <c r="G65" s="61" t="s">
+        <v>9</v>
+      </c>
+      <c r="H65" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="I65" s="25"/>
       <c r="J65" s="29"/>
       <c r="K65" s="8"/>
       <c r="L65" s="30"/>
       <c r="M65" s="8"/>
       <c r="N65" s="9"/>
-      <c r="O65" s="8"/>
-      <c r="P65" s="29"/>
+      <c r="O65" s="60" t="s">
+        <v>9</v>
+      </c>
+      <c r="P65" s="29" t="s">
+        <v>9</v>
+      </c>
       <c r="Q65" s="8"/>
       <c r="R65" s="30"/>
       <c r="S65" s="8"/>
@@ -10586,10 +10587,10 @@
     </row>
     <row r="66" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B66" s="75">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="C66" s="8">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D66" s="39">
         <v>20</v>
@@ -10619,10 +10620,10 @@
     </row>
     <row r="67" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B67" s="75">
-        <v>145</v>
+        <v>28</v>
       </c>
       <c r="C67" s="8">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D67" s="39">
         <v>20</v>
@@ -10651,11 +10652,21 @@
       <c r="V67" s="20"/>
     </row>
     <row r="68" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B68" s="37"/>
-      <c r="C68" s="8"/>
-      <c r="D68" s="39"/>
-      <c r="E68" s="49"/>
-      <c r="F68" s="57"/>
+      <c r="B68" s="75">
+        <v>145</v>
+      </c>
+      <c r="C68" s="8">
+        <v>11</v>
+      </c>
+      <c r="D68" s="39">
+        <v>20</v>
+      </c>
+      <c r="E68" s="49">
+        <v>44179</v>
+      </c>
+      <c r="F68" s="57">
+        <v>44200</v>
+      </c>
       <c r="G68" s="6"/>
       <c r="H68" s="7"/>
       <c r="I68" s="25"/>
@@ -10673,46 +10684,51 @@
       <c r="U68" s="10"/>
       <c r="V68" s="20"/>
     </row>
-    <row r="69" spans="2:22" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B69" s="38"/>
-      <c r="C69" s="58"/>
-      <c r="D69" s="40"/>
-      <c r="E69" s="40"/>
-      <c r="F69" s="19"/>
-      <c r="G69" s="74"/>
-      <c r="H69" s="53"/>
-      <c r="I69" s="54"/>
-      <c r="J69" s="55"/>
-      <c r="K69" s="72"/>
-      <c r="L69" s="31"/>
-      <c r="M69" s="72"/>
-      <c r="N69" s="19"/>
-      <c r="O69" s="72"/>
-      <c r="P69" s="31"/>
-      <c r="Q69" s="58"/>
-      <c r="R69" s="31"/>
-      <c r="S69" s="58"/>
-      <c r="T69" s="35"/>
-      <c r="U69" s="21"/>
-      <c r="V69" s="22"/>
+    <row r="69" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B69" s="37"/>
+      <c r="C69" s="8"/>
+      <c r="D69" s="39"/>
+      <c r="E69" s="49"/>
+      <c r="F69" s="57"/>
+      <c r="G69" s="6"/>
+      <c r="H69" s="7"/>
+      <c r="I69" s="25"/>
+      <c r="J69" s="29"/>
+      <c r="K69" s="8"/>
+      <c r="L69" s="30"/>
+      <c r="M69" s="8"/>
+      <c r="N69" s="9"/>
+      <c r="O69" s="8"/>
+      <c r="P69" s="29"/>
+      <c r="Q69" s="8"/>
+      <c r="R69" s="30"/>
+      <c r="S69" s="8"/>
+      <c r="T69" s="34"/>
+      <c r="U69" s="10"/>
+      <c r="V69" s="20"/>
     </row>
-    <row r="70" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="G70" s="8"/>
-      <c r="H70" s="8"/>
-      <c r="I70" s="8"/>
-      <c r="J70" s="8"/>
-      <c r="K70" s="8"/>
-      <c r="L70" s="8"/>
-      <c r="M70" s="8"/>
-      <c r="N70" s="8"/>
-      <c r="O70" s="8"/>
-      <c r="P70" s="8"/>
-      <c r="Q70" s="8"/>
-      <c r="R70" s="8"/>
-      <c r="S70" s="8"/>
-      <c r="T70" s="10"/>
-      <c r="U70" s="10"/>
-      <c r="V70" s="10"/>
+    <row r="70" spans="2:22" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B70" s="38"/>
+      <c r="C70" s="58"/>
+      <c r="D70" s="40"/>
+      <c r="E70" s="40"/>
+      <c r="F70" s="19"/>
+      <c r="G70" s="74"/>
+      <c r="H70" s="53"/>
+      <c r="I70" s="54"/>
+      <c r="J70" s="55"/>
+      <c r="K70" s="72"/>
+      <c r="L70" s="31"/>
+      <c r="M70" s="72"/>
+      <c r="N70" s="19"/>
+      <c r="O70" s="72"/>
+      <c r="P70" s="31"/>
+      <c r="Q70" s="58"/>
+      <c r="R70" s="31"/>
+      <c r="S70" s="58"/>
+      <c r="T70" s="35"/>
+      <c r="U70" s="21"/>
+      <c r="V70" s="22"/>
     </row>
     <row r="71" spans="2:22" x14ac:dyDescent="0.3">
       <c r="G71" s="8"/>
@@ -10769,7 +10785,6 @@
       <c r="V73" s="10"/>
     </row>
     <row r="74" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="F74" s="8"/>
       <c r="G74" s="8"/>
       <c r="H74" s="8"/>
       <c r="I74" s="8"/>
@@ -10839,6 +10854,25 @@
       <c r="P77" s="8"/>
       <c r="Q77" s="8"/>
       <c r="R77" s="8"/>
+      <c r="S77" s="8"/>
+      <c r="T77" s="10"/>
+      <c r="U77" s="10"/>
+      <c r="V77" s="10"/>
+    </row>
+    <row r="78" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="F78" s="8"/>
+      <c r="G78" s="8"/>
+      <c r="H78" s="8"/>
+      <c r="I78" s="8"/>
+      <c r="J78" s="8"/>
+      <c r="K78" s="8"/>
+      <c r="L78" s="8"/>
+      <c r="M78" s="8"/>
+      <c r="N78" s="8"/>
+      <c r="O78" s="8"/>
+      <c r="P78" s="8"/>
+      <c r="Q78" s="8"/>
+      <c r="R78" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="41">

</xml_diff>